<commit_message>
Added Dynamodb table to serverless config.
</commit_message>
<xml_diff>
--- a/dynamo_and_apis.xlsx
+++ b/dynamo_and_apis.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\bubblecheck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33B799F-BF67-40E0-80C7-1F8C5FBCEDDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D580CB-D7CB-4445-BE7E-18E0BAA49E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18510" yWindow="3945" windowWidth="28290" windowHeight="15555" xr2:uid="{4928332B-CF7E-41CC-9BAE-88DC4A418B31}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{4928332B-CF7E-41CC-9BAE-88DC4A418B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -427,7 +426,7 @@
             <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>/api/courses/my_courses [GET]</a:t>
+            <a:t>/api/courses [GET] (get just my courses)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -475,7 +474,7 @@
             <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>[ ] /api/courses/&lt;courseid&gt; [PUT]</a:t>
+            <a:t>[X] /api/courses/&lt;courseid&gt; [PUT]</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -540,7 +539,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>[ ] /api/courses/&lt;courseid&gt;/exams [POST]</a:t>
+            <a:t>[X] /api/courses/&lt;courseid&gt;/exams [POST]</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -571,7 +570,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>[ ] </a:t>
+            <a:t>[X] </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -591,7 +590,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>[ ] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt; [</a:t>
+            <a:t>[X] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt; [</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -628,21 +627,21 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>[ ] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt; [DELETE]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>[ ] /api/courses/&lt;courseid&gt;/permissions/&lt;usersid&gt; [GET]</a:t>
+            <a:t>[X] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt; [DELETE]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>[X] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt;/studentexams [POST]</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -650,17 +649,18 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>[ ] /api/courses/&lt;courseid&gt;/permissions/&lt;usersid&gt; [PUT]</a:t>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>[X] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt;/studentexams/&lt;studentexamid&gt; [PUT]</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -668,6 +668,39 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>[ ] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt;/studentexams/&lt;studentexamid&gt; [DELETE]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>[ ] /api/courses/&lt;courseid&gt;/permissions/&lt;usersid&gt; [PUT]</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:solidFill>
@@ -760,103 +793,6 @@
             <a:t>[ ] /api/courses/&lt;courseid&gt;/sections/&lt;sectionid&gt; [DELETE]</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>[ ] </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>/api/courses/&lt;courseid&gt;/exams/&lt;examid&gt;/studentexams [GET]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-            </a:rPr>
-            <a:t>[ ] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt;/studentexams [POST]</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>[ ] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt;/studentexams/&lt;studentexamid&gt; [PUT]</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
-            <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>[ ] /api/courses/&lt;courseid&gt;/exams/&lt;examid&gt;/studentexams/&lt;studentexamid&gt; [DELETE]</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
             <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
           </a:endParaRPr>
         </a:p>
@@ -1167,7 +1103,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>